<commit_message>
se actualizar la función editarUsuario
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556FC905-69F1-4C8B-AE92-408E3E480C19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC9BA6-6859-4693-B572-BD73D70AC339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -71,34 +71,35 @@
         2. Cuantas veces dio él examen de cada curso un profesor determinado.</t>
   </si>
   <si>
-    <t>Reporte gráfico para el docente, admin: determinar el número de alumnos que han:
+    <t>Solo tiene que ver su curso y acceder a ese examen simulador</t>
+  </si>
+  <si>
+    <t>Crear log(bitacora) para saber que es lo que esta modificando el profesor</t>
+  </si>
+  <si>
+    <t>25/04/2020
+(10 am 1pm)</t>
+  </si>
+  <si>
+    <t>27/04/2020
+(10am - 1pm,
+4pm - 8pm)</t>
+  </si>
+  <si>
+    <t>26/04/2020
+(10am - 1pm,
+4pm - 8pm))</t>
+  </si>
+  <si>
+    <t>28/04/2020
+(10am - 1pm,
+4pm - 8pm)</t>
+  </si>
+  <si>
+    <t>Reporte gráfico para el docente, admin: determinar el número de alumnos que han: (crear una tabla datoEstadistico relacionado con la tabla usuario)
         1. Dado el examen del simulador.
         2. Aprobado el examen simulador.
         3. Desaprobado el examen simulador.</t>
-  </si>
-  <si>
-    <t>Solo tiene que ver su curso y acceder a ese examen simulador</t>
-  </si>
-  <si>
-    <t>24/04/2020
-(10 am 1pm)</t>
-  </si>
-  <si>
-    <t>26/04/2020
-(10am - 1pm,
-4pm - 8pm)</t>
-  </si>
-  <si>
-    <t>25/04/2020
-(10 am - 1pm,
-4pm a 9pm)</t>
-  </si>
-  <si>
-    <t>24/04/2020
-(4pm - 6pm)</t>
-  </si>
-  <si>
-    <t>Crear log(bitacora) para saber que es lo que esta modificando el profesor</t>
   </si>
 </sst>
 </file>
@@ -164,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -296,11 +303,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,13 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -362,37 +389,46 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -407,8 +443,11 @@
     <xf numFmtId="9" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,7 +766,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,32 +782,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -794,30 +833,30 @@
       <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="34">
-        <v>0</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
+      <c r="D6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="19">
+      <c r="C7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="17">
         <v>0.3</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="13"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -826,49 +865,49 @@
       <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="17">
         <v>0.2</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="35"/>
-    </row>
-    <row r="9" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="30"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="36"/>
+    </row>
+    <row r="9" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <v>1</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="35"/>
-    </row>
-    <row r="10" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="F9" s="38"/>
+      <c r="G9" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="19">
+        <v>18</v>
+      </c>
+      <c r="D10" s="17">
         <v>1.5</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
@@ -877,28 +916,32 @@
       <c r="C11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="36"/>
+      <c r="E11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>6</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="C12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="25">
-        <v>43939</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="17">
+      <c r="E12" s="26">
+        <v>43949</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="19">
         <v>0</v>
       </c>
     </row>
@@ -909,18 +952,18 @@
         <v>5</v>
       </c>
       <c r="E13" s="7">
-        <v>43938</v>
+        <v>43946</v>
       </c>
       <c r="F13" s="8">
-        <v>43971</v>
+        <v>43979</v>
       </c>
       <c r="G13" s="9">
-        <f>SUM(G6:G12)/2</f>
-        <v>0</v>
+        <f>SUM(G6:G12)/4</f>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E7:F8"/>
@@ -928,7 +971,9 @@
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="G6:G11"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se agregó el módulo gestionarPreguntaDocente
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC9BA6-6859-4693-B572-BD73D70AC339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98CD7F-3625-4630-B83B-754B64F04E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agregó un nuevo archivo(reporteAlumno) para el menú, además ahora solo muestra la página principal el curso en donde esta inscrito el alumno
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98CD7F-3625-4630-B83B-754B64F04E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECAA3E3-5A5B-4BC4-A948-6913B15EC913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>CRONOGRAMA DE CORRECCIÓN</t>
   </si>
@@ -79,11 +79,6 @@
   <si>
     <t>25/04/2020
 (10 am 1pm)</t>
-  </si>
-  <si>
-    <t>27/04/2020
-(10am - 1pm,
-4pm - 8pm)</t>
   </si>
   <si>
     <t>26/04/2020
@@ -100,6 +95,22 @@
         1. Dado el examen del simulador.
         2. Aprobado el examen simulador.
         3. Desaprobado el examen simulador.</t>
+  </si>
+  <si>
+    <t>27/04/2020
+(6pm - 10pm)</t>
+  </si>
+  <si>
+    <t>Cuántos han iniciado sesión</t>
+  </si>
+  <si>
+    <t>Cuántos han dado el examen</t>
+  </si>
+  <si>
+    <t>cuántas veces han desaprobado</t>
+  </si>
+  <si>
+    <t>cuántas veces han aprobado</t>
   </si>
 </sst>
 </file>
@@ -763,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF9FE06-09A0-435C-B09F-75D423A945F8}">
-  <dimension ref="B1:J13"/>
+  <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,18 +890,18 @@
       <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -898,13 +909,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="17">
         <v>1.5</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="20"/>
@@ -920,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="21">
@@ -959,7 +970,27 @@
       </c>
       <c r="G13" s="9">
         <f>SUM(G6:G12)/4</f>
-        <v>0.25</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregó a la gráfica el número de alumnos que dierón el examen, desaprobados y aprobados.
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECAA3E3-5A5B-4BC4-A948-6913B15EC913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296A63C-B5AA-424C-BD07-D1484C74250B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,6 +459,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,7 +780,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +911,7 @@
       <c r="B10" s="10">
         <v>4</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="39" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="17">

</xml_diff>

<commit_message>
avance de los reportes para el admin con los docentes; además se avanzó con algunas correciones en reportes
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296A63C-B5AA-424C-BD07-D1484C74250B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CEA2AF-ACD8-49C5-84F6-E088CA776EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -415,6 +415,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,9 +462,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,7 +780,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,32 +796,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -849,12 +849,12 @@
       </c>
       <c r="D6" s="17"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="35">
+      <c r="G6" s="36">
         <v>1</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
@@ -866,11 +866,11 @@
       <c r="D7" s="17">
         <v>0.3</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="13"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -885,9 +885,9 @@
       <c r="D8" s="17">
         <v>0.2</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="36"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
@@ -899,10 +899,10 @@
       <c r="D9" s="17">
         <v>1</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="20">
         <v>1</v>
       </c>
@@ -911,16 +911,16 @@
       <c r="B10" s="10">
         <v>4</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="24" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="17">
         <v>1.5</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -933,10 +933,10 @@
       <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="21">
         <v>0</v>
       </c>
@@ -951,10 +951,10 @@
       <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="27">
         <v>43949</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="19">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
se termió con el log_pregunta
</commit_message>
<xml_diff>
--- a/mejoras del simulador(docente - admin y los reportes).xlsx
+++ b/mejoras del simulador(docente - admin y los reportes).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CampusVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CEA2AF-ACD8-49C5-84F6-E088CA776EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2B171F-A28B-44D6-AF27-DE332061F420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5748967-6E1D-4AFC-8929-D26A16BAFD2B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CRONOGRAMA DE CORRECCIÓN</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Solo tiene que ver su curso y acceder a ese examen simulador</t>
-  </si>
-  <si>
-    <t>Crear log(bitacora) para saber que es lo que esta modificando el profesor</t>
   </si>
   <si>
     <t>25/04/2020
@@ -101,16 +98,7 @@
 (6pm - 10pm)</t>
   </si>
   <si>
-    <t>Cuántos han iniciado sesión</t>
-  </si>
-  <si>
-    <t>Cuántos han dado el examen</t>
-  </si>
-  <si>
-    <t>cuántas veces han desaprobado</t>
-  </si>
-  <si>
-    <t>cuántas veces han aprobado</t>
+    <t>Crear log para todo lo que se puede gestionar, tanto para profesor, como para admin</t>
   </si>
 </sst>
 </file>
@@ -344,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,9 +372,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -777,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF9FE06-09A0-435C-B09F-75D423A945F8}">
-  <dimension ref="B1:J19"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,32 +781,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -847,30 +832,30 @@
       <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="36">
+      <c r="D6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="35">
         <v>1</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0.3</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="37"/>
+      <c r="E7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="13"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -879,31 +864,31 @@
       <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>0.2</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="37"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>1</v>
       </c>
-      <c r="E9" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="20">
+      <c r="E9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="19">
         <v>1</v>
       </c>
     </row>
@@ -911,33 +896,33 @@
       <c r="B10" s="10">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="20"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>1</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="21">
+      <c r="E11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="20">
         <v>0</v>
       </c>
     </row>
@@ -945,17 +930,17 @@
       <c r="B12" s="10">
         <v>6</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="15">
+      <c r="C12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="14">
         <v>1</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <v>43949</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="19">
+      <c r="F12" s="27"/>
+      <c r="G12" s="18">
         <v>0</v>
       </c>
     </row>
@@ -974,26 +959,6 @@
       <c r="G13" s="9">
         <f>SUM(G6:G12)/4</f>
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>